<commit_message>
Computed PCA m1 and RMap m1 for hatespeech
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/PCA/m1_results_PCA.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/PCA/m1_results_PCA.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1196,6 +1196,98 @@
         <v>0.9283685357187401</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:46:13</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>20</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.5007948904606515</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:46:13</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>10</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.6570267269092438</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:46:13</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>30</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.4054775467285684</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-10-02 16:46:13</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>hatespeech</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>40</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.3301035082478216</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>